<commit_message>
aims and objectives shit done
</commit_message>
<xml_diff>
--- a/doc/resourceAllocation/Table.xlsx
+++ b/doc/resourceAllocation/Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="243">
   <si>
     <t>Basic Tasks</t>
   </si>
@@ -747,6 +747,12 @@
   </si>
   <si>
     <t>A''13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impact </t>
+  </si>
+  <si>
+    <t>Utilisation</t>
   </si>
 </sst>
 </file>
@@ -1302,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35:R37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T33" sqref="T33:U34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2785,7 +2791,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
         <v>51</v>
@@ -2805,8 +2811,14 @@
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T33" t="s">
+        <v>241</v>
+      </c>
+      <c r="U33" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2820,8 +2832,16 @@
         <v>235</v>
       </c>
       <c r="R34" s="8"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T34" s="29">
+        <f>-0.326+0.234*AVERAGE(P2:P10)+0.436*AVERAGE(P12:P18)+0.585*AVERAGE(P20:P26)</f>
+        <v>0.68467289249032948</v>
+      </c>
+      <c r="U34" s="29">
+        <f>-0.326+0.234*AVERAGE(R2:R10)+0.436*AVERAGE(R12:R18)+0.585*AVERAGE(R20:R26)</f>
+        <v>0.81148650793650789</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
         <v>52</v>
@@ -2850,7 +2870,7 @@
         <v>0.9880000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
         <v>41</v>
@@ -2879,7 +2899,7 @@
         <v>0.87302777777777774</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
         <v>54</v>
@@ -2908,7 +2928,7 @@
         <v>0.94166666666666654</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
         <v>56</v>
@@ -2923,7 +2943,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
@@ -2940,7 +2960,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="3" t="s">
         <v>60</v>
@@ -2955,7 +2975,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
         <v>61</v>
@@ -2970,14 +2990,14 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="3" t="s">
         <v>62</v>
@@ -2992,7 +3012,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3" t="s">
         <v>63</v>
@@ -3007,14 +3027,14 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
         <v>64</v>

</xml_diff>